<commit_message>
compares mini group and larger data group
</commit_message>
<xml_diff>
--- a/cEBM_networkLabels.xlsx
+++ b/cEBM_networkLabels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brooke/Documents/WORK/cEBM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F10F5D3-59C9-AC46-B0E1-66BE260FAB3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67612780-4FF1-9B47-9A84-EF211E2A8BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9520" yWindow="700" windowWidth="27640" windowHeight="15640" xr2:uid="{AC3DC3E5-B104-E847-823D-FD784BCA6BE8}"/>
+    <workbookView xWindow="2380" yWindow="500" windowWidth="27640" windowHeight="15640" xr2:uid="{AC3DC3E5-B104-E847-823D-FD784BCA6BE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="11">
   <si>
     <t>AUD</t>
   </si>
@@ -64,6 +64,12 @@
   <si>
     <t>Nothing</t>
   </si>
+  <si>
+    <t>Small data analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Big Data analysis </t>
+  </si>
 </sst>
 </file>
 
@@ -86,7 +92,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,8 +135,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFEE0F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -195,11 +207,55 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -219,12 +275,25 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFEE0F2"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -234,6 +303,211 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE73F1E7-B0F3-3E7E-5D21-D13BEF1B5708}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6604000" y="381000"/>
+          <a:ext cx="6413500" cy="5156200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>790575</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>79375</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7382D2E7-7580-F194-CE11-B131798561D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13173075" y="396875"/>
+          <a:ext cx="6718300" cy="5146675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFFE89B4-D490-BCCA-FD76-1F99F86F2ECB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6604000" y="6238875"/>
+          <a:ext cx="6654800" cy="5092700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>184150</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>53975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2D5D48B-C568-AE82-6862-3DD0719A6A16}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13493750" y="6207125"/>
+          <a:ext cx="6502400" cy="5054600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -533,15 +807,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48B24107-92F5-4C4C-9EAB-BC565A79D7B5}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
@@ -555,7 +829,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -569,7 +843,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
@@ -583,7 +857,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>4</v>
       </c>
@@ -596,8 +870,12 @@
       <c r="D4" s="11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F4" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="24"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>5</v>
       </c>
@@ -610,8 +888,12 @@
       <c r="D5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F5" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="26"/>
+    </row>
+    <row r="6" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -625,7 +907,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>7</v>
       </c>
@@ -639,7 +921,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>8</v>
       </c>
@@ -653,7 +935,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>9</v>
       </c>
@@ -667,7 +949,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -681,21 +963,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+    <row r="11" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="19">
         <v>11</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="9">
+      <c r="B11" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="20">
         <v>2</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="21">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="13">
         <v>12</v>
       </c>
@@ -709,7 +991,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>13</v>
       </c>
@@ -723,7 +1005,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>14</v>
       </c>
@@ -737,7 +1019,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>15</v>
       </c>
@@ -751,7 +1033,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>16</v>
       </c>
@@ -892,16 +1174,16 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="A26" s="22">
         <v>26</v>
       </c>
-      <c r="B26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="4">
-        <v>4</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="B26" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="22">
+        <v>4</v>
+      </c>
+      <c r="D26" s="22" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1158,16 +1440,16 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45">
+      <c r="A45" s="22">
         <v>45</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C45" s="6">
-        <v>6</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="C45" s="22">
+        <v>6</v>
+      </c>
+      <c r="D45" s="22" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1229,5 +1511,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>